<commit_message>
Version for second submission
</commit_message>
<xml_diff>
--- a/experiments/3AU-IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/3AU-IISBMP2/data/biogas_and_setup.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="190">
   <si>
     <t xml:space="preserve">Experiment</t>
   </si>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
-    <t xml:space="preserve">LB</t>
+    <t xml:space="preserve">WS</t>
   </si>
   <si>
     <t xml:space="preserve">Substrate D</t>
@@ -635,6 +635,12 @@
   </si>
   <si>
     <t xml:space="preserve">Biogas sheet, mass.init column, copy out to vim, make new column, paste back in, to fix character/numeric issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Nove 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup sheet, change SC name to WS from LB</t>
   </si>
 </sst>
 </file>
@@ -742,7 +748,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -809,10 +815,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -902,9 +904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>77760</xdr:colOff>
+      <xdr:colOff>77400</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -914,7 +916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8010000" cy="1774440"/>
+          <a:ext cx="8003880" cy="1774080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -944,9 +946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>302040</xdr:colOff>
+      <xdr:colOff>301680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -956,7 +958,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5839560" cy="5101200"/>
+          <a:ext cx="5835600" cy="5100840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -991,9 +993,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>369360</xdr:colOff>
+      <xdr:colOff>369000</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>101880</xdr:rowOff>
+      <xdr:rowOff>101520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1003,7 +1005,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5775480" cy="4652280"/>
+          <a:ext cx="5775840" cy="4651920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1033,9 +1035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435960</xdr:colOff>
+      <xdr:colOff>435600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1045,7 +1047,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8845200" cy="9611280"/>
+          <a:ext cx="8845200" cy="9610920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1054,7 +1056,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1075,9 +1077,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435960</xdr:colOff>
+      <xdr:colOff>435600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1087,7 +1089,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8845200" cy="9611280"/>
+          <a:ext cx="8845200" cy="9610920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1096,7 +1098,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1117,9 +1119,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435960</xdr:colOff>
+      <xdr:colOff>435600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1129,7 +1131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8845200" cy="9611280"/>
+          <a:ext cx="8845200" cy="9610920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1138,7 +1140,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1159,9 +1161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>261720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1171,7 +1173,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5668200" cy="4654800"/>
+          <a:ext cx="5668560" cy="4654440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1210,7 +1212,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1219,7 +1221,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="1" width="9.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.88"/>
@@ -1227,7 +1229,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="1" width="9.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="9.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="1" width="9.46"/>
   </cols>
@@ -2313,18 +2315,18 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="9.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="8.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="9" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="9" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="7" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="8.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="7.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="12" width="9.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="12" width="9.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="14" style="12" width="7.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="12" width="5.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="5.35"/>
@@ -5373,7 +5375,7 @@
       <c r="C81" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="17" t="n">
+      <c r="D81" s="1" t="n">
         <v>8.07</v>
       </c>
       <c r="E81" s="9" t="n">
@@ -11638,19 +11640,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="8.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="48.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="12" width="8.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="12" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11668,7 +11670,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>145</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -11710,7 +11712,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>154</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -11724,7 +11726,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>156</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -11738,7 +11740,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>158</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -11752,7 +11754,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>158</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -11766,7 +11768,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>158</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -11780,7 +11782,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -11822,7 +11824,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>167</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -11836,7 +11838,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>169</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -11850,7 +11852,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>169</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -11864,7 +11866,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>169</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -11878,7 +11880,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>169</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -11892,7 +11894,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>174</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -11906,7 +11908,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>174</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -11920,7 +11922,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>174</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -11934,7 +11936,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>178</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -11948,7 +11950,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>180</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -11962,7 +11964,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>182</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -11976,7 +11978,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>184</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -12001,6 +12003,20 @@
       </c>
       <c r="D25" s="12" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct m.sub.vs in AU data, base on average of 3 labs as described in manuscript. Proof correction version.
</commit_message>
<xml_diff>
--- a/experiments/3AU-IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/3AU-IISBMP2/data/biogas_and_setup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">c.inoc.vs</t>
   </si>
   <si>
-    <t xml:space="preserve">m.sub.vs</t>
+    <t xml:space="preserve">m.sub.vs.rep</t>
   </si>
   <si>
     <t xml:space="preserve">m.inoc.vs</t>
@@ -904,9 +904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>77400</xdr:colOff>
+      <xdr:colOff>77040</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -916,7 +916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8003880" cy="1774080"/>
+          <a:ext cx="8002800" cy="1773720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -946,9 +946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
+      <xdr:colOff>301320</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -958,7 +958,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5835600" cy="5100840"/>
+          <a:ext cx="5835240" cy="5100480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,9 +993,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>369000</xdr:colOff>
+      <xdr:colOff>368640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1005,7 +1005,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5775840" cy="4651920"/>
+          <a:ext cx="5776200" cy="4651560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1035,9 +1035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435600</xdr:colOff>
+      <xdr:colOff>435240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1047,7 +1047,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8845200" cy="9610920"/>
+          <a:ext cx="8846280" cy="9610560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1077,9 +1077,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435600</xdr:colOff>
+      <xdr:colOff>435240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1089,7 +1089,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8845200" cy="9610920"/>
+          <a:ext cx="8846280" cy="9610560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1119,9 +1119,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435600</xdr:colOff>
+      <xdr:colOff>435240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1131,7 +1131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8845200" cy="9610920"/>
+          <a:ext cx="8846280" cy="9610560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1161,9 +1161,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>261720</xdr:colOff>
+      <xdr:colOff>261360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1173,7 +1173,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5668560" cy="4654440"/>
+          <a:ext cx="5668920" cy="4654080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1207,12 +1207,12 @@
   </sheetPr>
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11642,7 +11642,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>